<commit_message>
Major refactor of documents, everything should be much easier to find now
</commit_message>
<xml_diff>
--- a/documents/Risk Table.xlsx
+++ b/documents/Risk Table.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855" tabRatio="289"/>
   </bookViews>
   <sheets>
-    <sheet name="version 1.0" sheetId="1" r:id="rId1"/>
+    <sheet name="Sp2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sp1" sheetId="1" r:id="rId2"/>
+    <sheet name="Orig" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="37">
   <si>
     <t>NOAA permenantly goes offline</t>
   </si>
@@ -79,15 +81,9 @@
     <t>try to space our milestones out in a way that gives us enough time complete them, meet at least once a week to make sure everyone is on track</t>
   </si>
   <si>
-    <t>can't get a server from ITS</t>
-  </si>
-  <si>
     <t>use a free account from another email service</t>
   </si>
   <si>
-    <t>Use backup server for development</t>
-  </si>
-  <si>
     <t>website is not user friendly</t>
   </si>
   <si>
@@ -119,6 +115,18 @@
   </si>
   <si>
     <t>Contingency Plan</t>
+  </si>
+  <si>
+    <t>Limited Web API knowledge</t>
+  </si>
+  <si>
+    <t>Learn Web API</t>
+  </si>
+  <si>
+    <t>cannot get server from ITS</t>
+  </si>
+  <si>
+    <t>find a different server host</t>
   </si>
 </sst>
 </file>
@@ -189,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -220,11 +228,275 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -359,9 +631,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G11" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:G10" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:G10"/>
+  <sortState ref="A2:F12">
+    <sortCondition descending="1" ref="D1:D12"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="7" name="No." dataDxfId="17"/>
+    <tableColumn id="1" name="Risk" dataDxfId="13"/>
+    <tableColumn id="2" name="Likelihood" dataDxfId="12"/>
+    <tableColumn id="3" name="Impact" dataDxfId="11"/>
+    <tableColumn id="4" name="Score" dataDxfId="9">
+      <calculatedColumnFormula>PRODUCT(C2,D2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Mitigation Strategy" dataDxfId="10"/>
+    <tableColumn id="6" name="Contingency Plan" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G11" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:G11"/>
-  <sortState ref="B2:G12">
+  <sortState ref="A2:G11">
+    <sortCondition descending="1" ref="E1:E11"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="7" name="No." dataDxfId="24"/>
+    <tableColumn id="1" name="Risk" dataDxfId="23"/>
+    <tableColumn id="2" name="Likelihood" dataDxfId="22"/>
+    <tableColumn id="3" name="Impact" dataDxfId="21"/>
+    <tableColumn id="4" name="Score" dataDxfId="20">
+      <calculatedColumnFormula>PRODUCT(C2,D2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Mitigation Strategy" dataDxfId="19"/>
+    <tableColumn id="6" name="Contingency Plan" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:G12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G12"/>
+  <sortState ref="A2:G12">
     <sortCondition descending="1" ref="E1:E12"/>
   </sortState>
   <tableColumns count="7">
@@ -666,10 +980,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="7" max="7" width="51.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="12">
+        <v>10</v>
+      </c>
+      <c r="D2" s="12">
+        <v>10</v>
+      </c>
+      <c r="E2" s="13">
+        <f t="shared" ref="E2:E10" si="0">PRODUCT(C2,D2)</f>
+        <v>100</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>3</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="12">
+        <v>5</v>
+      </c>
+      <c r="D3" s="12">
+        <v>7</v>
+      </c>
+      <c r="E3" s="13">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>4</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="12">
+        <v>4</v>
+      </c>
+      <c r="D4" s="12">
+        <v>8</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>6</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="12">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12">
+        <v>4</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>7</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="12">
+        <v>4</v>
+      </c>
+      <c r="D6" s="12">
+        <v>4</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>8</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="12">
+        <v>2</v>
+      </c>
+      <c r="D7" s="12">
+        <v>6</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>9</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="12">
+        <v>1</v>
+      </c>
+      <c r="D8" s="12">
+        <v>10</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>10</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12">
+        <v>10</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>11</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="12">
+        <v>1</v>
+      </c>
+      <c r="D10" s="12">
+        <v>8</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E10">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -691,25 +1303,25 @@
   <sheetData>
     <row r="1" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="N1" s="1"/>
     </row>
@@ -727,7 +1339,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="10">
-        <f t="shared" ref="E2:E11" si="0">PRODUCT(C2,D2)</f>
+        <f>PRODUCT(C2,D2)</f>
         <v>100</v>
       </c>
       <c r="F2" s="9" t="s">
@@ -738,84 +1350,84 @@
       </c>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C3" s="11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3" s="11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E3" s="10">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <f>PRODUCT(C3,D3)</f>
+        <v>90</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C4" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="10">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <f>PRODUCT(C4,D4)</f>
+        <v>35</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C5" s="11">
         <v>4</v>
       </c>
       <c r="D5" s="11">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E5" s="10">
-        <f t="shared" si="0"/>
+        <f>PRODUCT(C5,D5)</f>
+        <v>32</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>1</v>
-      </c>
       <c r="G5" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>7</v>
@@ -827,7 +1439,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="10">
-        <f t="shared" si="0"/>
+        <f>PRODUCT(C6,D6)</f>
         <v>20</v>
       </c>
       <c r="F6" s="9" t="s">
@@ -840,7 +1452,7 @@
     </row>
     <row r="7" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>9</v>
@@ -852,20 +1464,20 @@
         <v>4</v>
       </c>
       <c r="E7" s="10">
-        <f t="shared" si="0"/>
+        <f>PRODUCT(C7,D7)</f>
         <v>16</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>5</v>
@@ -877,7 +1489,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="10">
-        <f t="shared" si="0"/>
+        <f>PRODUCT(C8,D8)</f>
         <v>12</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -890,7 +1502,7 @@
     </row>
     <row r="9" spans="1:14" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>0</v>
@@ -902,20 +1514,20 @@
         <v>10</v>
       </c>
       <c r="E9" s="10">
-        <f t="shared" si="0"/>
+        <f>PRODUCT(C9,D9)</f>
         <v>10</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>17</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>3</v>
@@ -927,7 +1539,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="10">
-        <f t="shared" si="0"/>
+        <f>PRODUCT(C10,D10)</f>
         <v>10</v>
       </c>
       <c r="F10" s="9" t="s">
@@ -941,7 +1553,7 @@
     </row>
     <row r="11" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>6</v>
@@ -953,7 +1565,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="10">
-        <f t="shared" si="0"/>
+        <f>PRODUCT(C11,D11)</f>
         <v>8</v>
       </c>
       <c r="F11" s="9" t="s">
@@ -1194,4 +1806,378 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="6" max="6" width="61.7109375" customWidth="1"/>
+    <col min="7" max="7" width="60.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="11">
+        <v>10</v>
+      </c>
+      <c r="D2" s="11">
+        <v>10</v>
+      </c>
+      <c r="E2" s="10">
+        <f>PRODUCT(C2,D2)</f>
+        <v>100</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="11">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11">
+        <v>9</v>
+      </c>
+      <c r="E3" s="10">
+        <f>PRODUCT(C3,D3)</f>
+        <v>90</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="11">
+        <v>5</v>
+      </c>
+      <c r="D4" s="11">
+        <v>7</v>
+      </c>
+      <c r="E4" s="10">
+        <f>PRODUCT(C4,D4)</f>
+        <v>35</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="11">
+        <v>4</v>
+      </c>
+      <c r="D5" s="11">
+        <v>8</v>
+      </c>
+      <c r="E5" s="10">
+        <f>PRODUCT(C5,D5)</f>
+        <v>32</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="11">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11">
+        <v>6</v>
+      </c>
+      <c r="E6" s="10">
+        <f>PRODUCT(C6,D6)</f>
+        <v>24</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="11">
+        <v>5</v>
+      </c>
+      <c r="D7" s="11">
+        <v>4</v>
+      </c>
+      <c r="E7" s="10">
+        <f>PRODUCT(C7,D7)</f>
+        <v>20</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="11">
+        <v>4</v>
+      </c>
+      <c r="D8" s="11">
+        <v>4</v>
+      </c>
+      <c r="E8" s="10">
+        <f>PRODUCT(C8,D8)</f>
+        <v>16</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="11">
+        <v>2</v>
+      </c>
+      <c r="D9" s="11">
+        <v>6</v>
+      </c>
+      <c r="E9" s="10">
+        <f>PRODUCT(C9,D9)</f>
+        <v>12</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="11">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11">
+        <v>10</v>
+      </c>
+      <c r="E10" s="10">
+        <f>PRODUCT(C10,D10)</f>
+        <v>10</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="11">
+        <v>10</v>
+      </c>
+      <c r="E11" s="10">
+        <f>PRODUCT(C11,D11)</f>
+        <v>10</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="11">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11">
+        <v>8</v>
+      </c>
+      <c r="E12" s="10">
+        <f>PRODUCT(C12,D12)</f>
+        <v>8</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E6 E8:E12">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>